<commit_message>
Added much diverse datasets
</commit_message>
<xml_diff>
--- a/Datasets/Sales.xlsx
+++ b/Datasets/Sales.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21901"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\R Course\Datasets\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8E90665-89BA-4626-920F-BCE692CA2B11}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="20055" windowHeight="7935"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,13 +26,13 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Chris Albright</author>
     <author>SAMSUNG</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0">
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -50,7 +56,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B1" authorId="0">
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -74,7 +80,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0">
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
       <text>
         <r>
           <rPr>
@@ -98,7 +104,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D1" authorId="0">
+    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
       <text>
         <r>
           <rPr>
@@ -122,7 +128,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E1" authorId="0">
+    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
       <text>
         <r>
           <rPr>
@@ -146,7 +152,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="0">
+    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000006000000}">
       <text>
         <r>
           <rPr>
@@ -170,7 +176,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G1" authorId="0">
+    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000007000000}">
       <text>
         <r>
           <rPr>
@@ -194,7 +200,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H1" authorId="0">
+    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000008000000}">
       <text>
         <r>
           <rPr>
@@ -218,7 +224,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I1" authorId="0">
+    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000009000000}">
       <text>
         <r>
           <rPr>
@@ -242,7 +248,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J1" authorId="0">
+    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000A000000}">
       <text>
         <r>
           <rPr>
@@ -266,7 +272,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I10" authorId="1">
+    <comment ref="I10" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000B000000}">
       <text>
         <r>
           <rPr>
@@ -280,7 +286,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I43" authorId="1">
+    <comment ref="I43" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000C000000}">
       <text>
         <r>
           <rPr>
@@ -294,7 +300,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I312" authorId="1">
+    <comment ref="I312" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000D000000}">
       <text>
         <r>
           <rPr>
@@ -411,11 +417,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="7" formatCode="&quot;$&quot;#,##0.00_);\(&quot;$&quot;#,##0.00\)"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00_);\(&quot;$&quot;#,##0.00\)"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -469,14 +475,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="7" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="7" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -484,6 +490,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -530,7 +544,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -562,9 +576,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -596,6 +628,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -771,14 +821,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W404"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5.85546875" bestFit="1" customWidth="1"/>
@@ -792,7 +845,7 @@
     <col min="13" max="13" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -833,7 +886,7 @@
       <c r="V1" s="5"/>
       <c r="W1" s="5"/>
     </row>
-    <row r="2" spans="1:23">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>38782</v>
       </c>
@@ -875,7 +928,7 @@
       <c r="V2" s="5"/>
       <c r="W2" s="5"/>
     </row>
-    <row r="3" spans="1:23">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>38782</v>
       </c>
@@ -917,7 +970,7 @@
       <c r="V3" s="5"/>
       <c r="W3" s="5"/>
     </row>
-    <row r="4" spans="1:23">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>38782</v>
       </c>
@@ -959,7 +1012,7 @@
       <c r="V4" s="5"/>
       <c r="W4" s="5"/>
     </row>
-    <row r="5" spans="1:23">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>38782</v>
       </c>
@@ -1000,7 +1053,7 @@
       <c r="V5" s="5"/>
       <c r="W5" s="5"/>
     </row>
-    <row r="6" spans="1:23">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>38782</v>
       </c>
@@ -1041,7 +1094,7 @@
       <c r="V6" s="5"/>
       <c r="W6" s="5"/>
     </row>
-    <row r="7" spans="1:23">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>38782</v>
       </c>
@@ -1082,7 +1135,7 @@
       <c r="V7" s="5"/>
       <c r="W7" s="5"/>
     </row>
-    <row r="8" spans="1:23">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>38783</v>
       </c>
@@ -1123,7 +1176,7 @@
       <c r="V8" s="5"/>
       <c r="W8" s="5"/>
     </row>
-    <row r="9" spans="1:23">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>38783</v>
       </c>
@@ -1164,7 +1217,7 @@
       <c r="V9" s="5"/>
       <c r="W9" s="5"/>
     </row>
-    <row r="10" spans="1:23">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>38784</v>
       </c>
@@ -1205,7 +1258,7 @@
       <c r="V10" s="5"/>
       <c r="W10" s="5"/>
     </row>
-    <row r="11" spans="1:23">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>38783</v>
       </c>
@@ -1246,7 +1299,7 @@
       <c r="V11" s="5"/>
       <c r="W11" s="5"/>
     </row>
-    <row r="12" spans="1:23">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>38784</v>
       </c>
@@ -1287,7 +1340,7 @@
       <c r="V12" s="5"/>
       <c r="W12" s="5"/>
     </row>
-    <row r="13" spans="1:23">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>38784</v>
       </c>
@@ -1328,7 +1381,7 @@
       <c r="V13" s="5"/>
       <c r="W13" s="5"/>
     </row>
-    <row r="14" spans="1:23">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>38784</v>
       </c>
@@ -1369,7 +1422,7 @@
       <c r="V14" s="5"/>
       <c r="W14" s="5"/>
     </row>
-    <row r="15" spans="1:23">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>38785</v>
       </c>
@@ -1410,7 +1463,7 @@
       <c r="V15" s="5"/>
       <c r="W15" s="5"/>
     </row>
-    <row r="16" spans="1:23">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>38785</v>
       </c>
@@ -1451,7 +1504,7 @@
       <c r="V16" s="5"/>
       <c r="W16" s="5"/>
     </row>
-    <row r="17" spans="1:23">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>38786</v>
       </c>
@@ -1492,7 +1545,7 @@
       <c r="V17" s="5"/>
       <c r="W17" s="5"/>
     </row>
-    <row r="18" spans="1:23">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>38786</v>
       </c>
@@ -1533,7 +1586,7 @@
       <c r="V18" s="5"/>
       <c r="W18" s="5"/>
     </row>
-    <row r="19" spans="1:23">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>38786</v>
       </c>
@@ -1574,7 +1627,7 @@
       <c r="V19" s="5"/>
       <c r="W19" s="5"/>
     </row>
-    <row r="20" spans="1:23">
+    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>38786</v>
       </c>
@@ -1615,7 +1668,7 @@
       <c r="V20" s="5"/>
       <c r="W20" s="5"/>
     </row>
-    <row r="21" spans="1:23">
+    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>38787</v>
       </c>
@@ -1656,7 +1709,7 @@
       <c r="V21" s="5"/>
       <c r="W21" s="5"/>
     </row>
-    <row r="22" spans="1:23">
+    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>38787</v>
       </c>
@@ -1697,7 +1750,7 @@
       <c r="V22" s="5"/>
       <c r="W22" s="5"/>
     </row>
-    <row r="23" spans="1:23">
+    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>38788</v>
       </c>
@@ -1738,7 +1791,7 @@
       <c r="V23" s="5"/>
       <c r="W23" s="5"/>
     </row>
-    <row r="24" spans="1:23">
+    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>38788</v>
       </c>
@@ -1779,7 +1832,7 @@
       <c r="V24" s="5"/>
       <c r="W24" s="5"/>
     </row>
-    <row r="25" spans="1:23">
+    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>38788</v>
       </c>
@@ -1820,7 +1873,7 @@
       <c r="V25" s="5"/>
       <c r="W25" s="5"/>
     </row>
-    <row r="26" spans="1:23">
+    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>38789</v>
       </c>
@@ -1861,7 +1914,7 @@
       <c r="V26" s="5"/>
       <c r="W26" s="5"/>
     </row>
-    <row r="27" spans="1:23">
+    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <v>38789</v>
       </c>
@@ -1902,7 +1955,7 @@
       <c r="V27" s="5"/>
       <c r="W27" s="5"/>
     </row>
-    <row r="28" spans="1:23">
+    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <v>38790</v>
       </c>
@@ -1943,7 +1996,7 @@
       <c r="V28" s="5"/>
       <c r="W28" s="5"/>
     </row>
-    <row r="29" spans="1:23">
+    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <v>38790</v>
       </c>
@@ -1984,7 +2037,7 @@
       <c r="V29" s="5"/>
       <c r="W29" s="5"/>
     </row>
-    <row r="30" spans="1:23">
+    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
         <v>38790</v>
       </c>
@@ -2025,7 +2078,7 @@
       <c r="V30" s="5"/>
       <c r="W30" s="5"/>
     </row>
-    <row r="31" spans="1:23">
+    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
         <v>38791</v>
       </c>
@@ -2066,7 +2119,7 @@
       <c r="V31" s="5"/>
       <c r="W31" s="5"/>
     </row>
-    <row r="32" spans="1:23">
+    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
         <v>38791</v>
       </c>
@@ -2107,7 +2160,7 @@
       <c r="V32" s="5"/>
       <c r="W32" s="5"/>
     </row>
-    <row r="33" spans="1:23">
+    <row r="33" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
         <v>38792</v>
       </c>
@@ -2148,7 +2201,7 @@
       <c r="V33" s="5"/>
       <c r="W33" s="5"/>
     </row>
-    <row r="34" spans="1:23">
+    <row r="34" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
         <v>38792</v>
       </c>
@@ -2189,7 +2242,7 @@
       <c r="V34" s="5"/>
       <c r="W34" s="5"/>
     </row>
-    <row r="35" spans="1:23">
+    <row r="35" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
         <v>38792</v>
       </c>
@@ -2230,7 +2283,7 @@
       <c r="V35" s="5"/>
       <c r="W35" s="5"/>
     </row>
-    <row r="36" spans="1:23">
+    <row r="36" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A36" s="3">
         <v>38792</v>
       </c>
@@ -2271,7 +2324,7 @@
       <c r="V36" s="5"/>
       <c r="W36" s="5"/>
     </row>
-    <row r="37" spans="1:23">
+    <row r="37" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A37" s="3">
         <v>38793</v>
       </c>
@@ -2312,7 +2365,7 @@
       <c r="V37" s="5"/>
       <c r="W37" s="5"/>
     </row>
-    <row r="38" spans="1:23">
+    <row r="38" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A38" s="3">
         <v>38793</v>
       </c>
@@ -2353,7 +2406,7 @@
       <c r="V38" s="5"/>
       <c r="W38" s="5"/>
     </row>
-    <row r="39" spans="1:23">
+    <row r="39" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A39" s="3">
         <v>38793</v>
       </c>
@@ -2394,7 +2447,7 @@
       <c r="V39" s="5"/>
       <c r="W39" s="5"/>
     </row>
-    <row r="40" spans="1:23">
+    <row r="40" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A40" s="3">
         <v>38794</v>
       </c>
@@ -2435,7 +2488,7 @@
       <c r="V40" s="5"/>
       <c r="W40" s="5"/>
     </row>
-    <row r="41" spans="1:23">
+    <row r="41" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A41" s="3">
         <v>38794</v>
       </c>
@@ -2476,7 +2529,7 @@
       <c r="V41" s="5"/>
       <c r="W41" s="5"/>
     </row>
-    <row r="42" spans="1:23">
+    <row r="42" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A42" s="3">
         <v>38794</v>
       </c>
@@ -2517,7 +2570,7 @@
       <c r="V42" s="5"/>
       <c r="W42" s="5"/>
     </row>
-    <row r="43" spans="1:23">
+    <row r="43" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A43" s="3">
         <v>38794</v>
       </c>
@@ -2558,7 +2611,7 @@
       <c r="V43" s="5"/>
       <c r="W43" s="5"/>
     </row>
-    <row r="44" spans="1:23">
+    <row r="44" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A44" s="3">
         <v>38794</v>
       </c>
@@ -2599,7 +2652,7 @@
       <c r="V44" s="5"/>
       <c r="W44" s="5"/>
     </row>
-    <row r="45" spans="1:23">
+    <row r="45" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A45" s="3">
         <v>38794</v>
       </c>
@@ -2640,7 +2693,7 @@
       <c r="V45" s="5"/>
       <c r="W45" s="5"/>
     </row>
-    <row r="46" spans="1:23">
+    <row r="46" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A46" s="3">
         <v>38794</v>
       </c>
@@ -2681,7 +2734,7 @@
       <c r="V46" s="5"/>
       <c r="W46" s="5"/>
     </row>
-    <row r="47" spans="1:23">
+    <row r="47" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A47" s="3">
         <v>38794</v>
       </c>
@@ -2722,7 +2775,7 @@
       <c r="V47" s="5"/>
       <c r="W47" s="5"/>
     </row>
-    <row r="48" spans="1:23">
+    <row r="48" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A48" s="3">
         <v>38795</v>
       </c>
@@ -2763,7 +2816,7 @@
       <c r="V48" s="5"/>
       <c r="W48" s="5"/>
     </row>
-    <row r="49" spans="1:23">
+    <row r="49" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A49" s="3">
         <v>38796</v>
       </c>
@@ -2804,7 +2857,7 @@
       <c r="V49" s="5"/>
       <c r="W49" s="5"/>
     </row>
-    <row r="50" spans="1:23">
+    <row r="50" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A50" s="3">
         <v>38796</v>
       </c>
@@ -2845,7 +2898,7 @@
       <c r="V50" s="5"/>
       <c r="W50" s="5"/>
     </row>
-    <row r="51" spans="1:23">
+    <row r="51" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A51" s="3">
         <v>38796</v>
       </c>
@@ -2886,7 +2939,7 @@
       <c r="V51" s="5"/>
       <c r="W51" s="5"/>
     </row>
-    <row r="52" spans="1:23">
+    <row r="52" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A52" s="3">
         <v>38796</v>
       </c>
@@ -2927,7 +2980,7 @@
       <c r="V52" s="5"/>
       <c r="W52" s="5"/>
     </row>
-    <row r="53" spans="1:23">
+    <row r="53" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A53" s="3">
         <v>38796</v>
       </c>
@@ -2968,7 +3021,7 @@
       <c r="V53" s="5"/>
       <c r="W53" s="5"/>
     </row>
-    <row r="54" spans="1:23">
+    <row r="54" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A54" s="3">
         <v>38797</v>
       </c>
@@ -3009,7 +3062,7 @@
       <c r="V54" s="5"/>
       <c r="W54" s="5"/>
     </row>
-    <row r="55" spans="1:23">
+    <row r="55" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A55" s="3">
         <v>38797</v>
       </c>
@@ -3050,7 +3103,7 @@
       <c r="V55" s="5"/>
       <c r="W55" s="5"/>
     </row>
-    <row r="56" spans="1:23">
+    <row r="56" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A56" s="3">
         <v>38797</v>
       </c>
@@ -3091,7 +3144,7 @@
       <c r="V56" s="5"/>
       <c r="W56" s="5"/>
     </row>
-    <row r="57" spans="1:23">
+    <row r="57" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A57" s="3">
         <v>38798</v>
       </c>
@@ -3132,7 +3185,7 @@
       <c r="V57" s="5"/>
       <c r="W57" s="5"/>
     </row>
-    <row r="58" spans="1:23">
+    <row r="58" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A58" s="3">
         <v>38799</v>
       </c>
@@ -3173,7 +3226,7 @@
       <c r="V58" s="5"/>
       <c r="W58" s="5"/>
     </row>
-    <row r="59" spans="1:23">
+    <row r="59" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A59" s="3">
         <v>38799</v>
       </c>
@@ -3214,7 +3267,7 @@
       <c r="V59" s="5"/>
       <c r="W59" s="5"/>
     </row>
-    <row r="60" spans="1:23">
+    <row r="60" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A60" s="3">
         <v>38800</v>
       </c>
@@ -3246,7 +3299,7 @@
         <v>24.31</v>
       </c>
     </row>
-    <row r="61" spans="1:23">
+    <row r="61" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A61" s="3">
         <v>38800</v>
       </c>
@@ -3278,7 +3331,7 @@
         <v>34.47</v>
       </c>
     </row>
-    <row r="62" spans="1:23">
+    <row r="62" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A62" s="3">
         <v>38800</v>
       </c>
@@ -3310,7 +3363,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="63" spans="1:23">
+    <row r="63" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A63" s="3">
         <v>38800</v>
       </c>
@@ -3342,7 +3395,7 @@
         <v>43.78</v>
       </c>
     </row>
-    <row r="64" spans="1:23">
+    <row r="64" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A64" s="3">
         <v>38801</v>
       </c>
@@ -3374,7 +3427,7 @@
         <v>53.39</v>
       </c>
     </row>
-    <row r="65" spans="1:10">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" s="3">
         <v>38801</v>
       </c>
@@ -3406,7 +3459,7 @@
         <v>29.05</v>
       </c>
     </row>
-    <row r="66" spans="1:10">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" s="3">
         <v>38801</v>
       </c>
@@ -3438,7 +3491,7 @@
         <v>80.58</v>
       </c>
     </row>
-    <row r="67" spans="1:10">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" s="3">
         <v>38801</v>
       </c>
@@ -3470,7 +3523,7 @@
         <v>38.159999999999997</v>
       </c>
     </row>
-    <row r="68" spans="1:10">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" s="3">
         <v>38801</v>
       </c>
@@ -3502,7 +3555,7 @@
         <v>85.34</v>
       </c>
     </row>
-    <row r="69" spans="1:10">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" s="3">
         <v>38801</v>
       </c>
@@ -3534,7 +3587,7 @@
         <v>39.57</v>
       </c>
     </row>
-    <row r="70" spans="1:10">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" s="3">
         <v>38801</v>
       </c>
@@ -3566,7 +3619,7 @@
         <v>28.87</v>
       </c>
     </row>
-    <row r="71" spans="1:10">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" s="3">
         <v>38801</v>
       </c>
@@ -3598,7 +3651,7 @@
         <v>114.81</v>
       </c>
     </row>
-    <row r="72" spans="1:10">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" s="3">
         <v>38801</v>
       </c>
@@ -3630,7 +3683,7 @@
         <v>44.84</v>
       </c>
     </row>
-    <row r="73" spans="1:10">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" s="3">
         <v>38801</v>
       </c>
@@ -3662,7 +3715,7 @@
         <v>63.21</v>
       </c>
     </row>
-    <row r="74" spans="1:10">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" s="3">
         <v>38802</v>
       </c>
@@ -3694,7 +3747,7 @@
         <v>37.24</v>
       </c>
     </row>
-    <row r="75" spans="1:10">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" s="3">
         <v>38802</v>
       </c>
@@ -3726,7 +3779,7 @@
         <v>21.23</v>
       </c>
     </row>
-    <row r="76" spans="1:10">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" s="3">
         <v>38803</v>
       </c>
@@ -3758,7 +3811,7 @@
         <v>308.27999999999997</v>
       </c>
     </row>
-    <row r="77" spans="1:10">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" s="3">
         <v>38803</v>
       </c>
@@ -3790,7 +3843,7 @@
         <v>111.98</v>
       </c>
     </row>
-    <row r="78" spans="1:10">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" s="3">
         <v>38803</v>
       </c>
@@ -3822,7 +3875,7 @@
         <v>102.31</v>
       </c>
     </row>
-    <row r="79" spans="1:10">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" s="3">
         <v>38803</v>
       </c>
@@ -3854,7 +3907,7 @@
         <v>32.51</v>
       </c>
     </row>
-    <row r="80" spans="1:10">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" s="3">
         <v>38804</v>
       </c>
@@ -3886,7 +3939,7 @@
         <v>62.58</v>
       </c>
     </row>
-    <row r="81" spans="1:10">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" s="3">
         <v>38804</v>
       </c>
@@ -3918,7 +3971,7 @@
         <v>160.86000000000001</v>
       </c>
     </row>
-    <row r="82" spans="1:10">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" s="3">
         <v>38804</v>
       </c>
@@ -3950,7 +4003,7 @@
         <v>77.42</v>
       </c>
     </row>
-    <row r="83" spans="1:10">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" s="3">
         <v>38804</v>
       </c>
@@ -3982,7 +4035,7 @@
         <v>81.14</v>
       </c>
     </row>
-    <row r="84" spans="1:10">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" s="3">
         <v>38805</v>
       </c>
@@ -4014,7 +4067,7 @@
         <v>59.3</v>
       </c>
     </row>
-    <row r="85" spans="1:10">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85" s="3">
         <v>38805</v>
       </c>
@@ -4046,7 +4099,7 @@
         <v>21.13</v>
       </c>
     </row>
-    <row r="86" spans="1:10">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86" s="3">
         <v>38805</v>
       </c>
@@ -4078,7 +4131,7 @@
         <v>87.54</v>
       </c>
     </row>
-    <row r="87" spans="1:10">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87" s="3">
         <v>38805</v>
       </c>
@@ -4110,7 +4163,7 @@
         <v>53.48</v>
       </c>
     </row>
-    <row r="88" spans="1:10">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88" s="3">
         <v>38806</v>
       </c>
@@ -4142,7 +4195,7 @@
         <v>30.51</v>
       </c>
     </row>
-    <row r="89" spans="1:10">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89" s="3">
         <v>38806</v>
       </c>
@@ -4174,7 +4227,7 @@
         <v>82.01</v>
       </c>
     </row>
-    <row r="90" spans="1:10">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90" s="3">
         <v>38806</v>
       </c>
@@ -4206,7 +4259,7 @@
         <v>33.72</v>
       </c>
     </row>
-    <row r="91" spans="1:10">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91" s="3">
         <v>38806</v>
       </c>
@@ -4238,7 +4291,7 @@
         <v>27.99</v>
       </c>
     </row>
-    <row r="92" spans="1:10">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92" s="3">
         <v>38807</v>
       </c>
@@ -4270,7 +4323,7 @@
         <v>82.34</v>
       </c>
     </row>
-    <row r="93" spans="1:10">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93" s="3">
         <v>38807</v>
       </c>
@@ -4302,7 +4355,7 @@
         <v>118.79</v>
       </c>
     </row>
-    <row r="94" spans="1:10">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94" s="3">
         <v>38808</v>
       </c>
@@ -4334,7 +4387,7 @@
         <v>26.05</v>
       </c>
     </row>
-    <row r="95" spans="1:10">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95" s="3">
         <v>38808</v>
       </c>
@@ -4366,7 +4419,7 @@
         <v>31.16</v>
       </c>
     </row>
-    <row r="96" spans="1:10">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96" s="3">
         <v>38808</v>
       </c>
@@ -4398,7 +4451,7 @@
         <v>65.11</v>
       </c>
     </row>
-    <row r="97" spans="1:10">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A97" s="3">
         <v>38808</v>
       </c>
@@ -4430,7 +4483,7 @@
         <v>68.61</v>
       </c>
     </row>
-    <row r="98" spans="1:10">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A98" s="3">
         <v>38808</v>
       </c>
@@ -4462,7 +4515,7 @@
         <v>37.619999999999997</v>
       </c>
     </row>
-    <row r="99" spans="1:10">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A99" s="3">
         <v>38809</v>
       </c>
@@ -4494,7 +4547,7 @@
         <v>64.91</v>
       </c>
     </row>
-    <row r="100" spans="1:10">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A100" s="3">
         <v>38809</v>
       </c>
@@ -4526,7 +4579,7 @@
         <v>37.950000000000003</v>
       </c>
     </row>
-    <row r="101" spans="1:10">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A101" s="3">
         <v>38809</v>
       </c>
@@ -4558,7 +4611,7 @@
         <v>102.77</v>
       </c>
     </row>
-    <row r="102" spans="1:10">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A102" s="3">
         <v>38809</v>
       </c>
@@ -4590,7 +4643,7 @@
         <v>58.11</v>
       </c>
     </row>
-    <row r="103" spans="1:10">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A103" s="3">
         <v>38810</v>
       </c>
@@ -4622,7 +4675,7 @@
         <v>38.1</v>
       </c>
     </row>
-    <row r="104" spans="1:10">
+    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A104" s="3">
         <v>38811</v>
       </c>
@@ -4654,7 +4707,7 @@
         <v>83.62</v>
       </c>
     </row>
-    <row r="105" spans="1:10">
+    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A105" s="3">
         <v>38811</v>
       </c>
@@ -4686,7 +4739,7 @@
         <v>191.95</v>
       </c>
     </row>
-    <row r="106" spans="1:10">
+    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A106" s="3">
         <v>38811</v>
       </c>
@@ -4718,7 +4771,7 @@
         <v>24.43</v>
       </c>
     </row>
-    <row r="107" spans="1:10">
+    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A107" s="3">
         <v>38811</v>
       </c>
@@ -4750,7 +4803,7 @@
         <v>52.83</v>
       </c>
     </row>
-    <row r="108" spans="1:10">
+    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A108" s="3">
         <v>38812</v>
       </c>
@@ -4782,7 +4835,7 @@
         <v>109.97</v>
       </c>
     </row>
-    <row r="109" spans="1:10">
+    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A109" s="3">
         <v>38812</v>
       </c>
@@ -4814,7 +4867,7 @@
         <v>74.959999999999994</v>
       </c>
     </row>
-    <row r="110" spans="1:10">
+    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A110" s="3">
         <v>38812</v>
       </c>
@@ -4846,7 +4899,7 @@
         <v>70.03</v>
       </c>
     </row>
-    <row r="111" spans="1:10">
+    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A111" s="3">
         <v>38812</v>
       </c>
@@ -4878,7 +4931,7 @@
         <v>102.86</v>
       </c>
     </row>
-    <row r="112" spans="1:10">
+    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A112" s="3">
         <v>38812</v>
       </c>
@@ -4910,7 +4963,7 @@
         <v>114.41</v>
       </c>
     </row>
-    <row r="113" spans="1:10">
+    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A113" s="3">
         <v>38813</v>
       </c>
@@ -4942,7 +4995,7 @@
         <v>31.19</v>
       </c>
     </row>
-    <row r="114" spans="1:10">
+    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A114" s="3">
         <v>38813</v>
       </c>
@@ -4974,7 +5027,7 @@
         <v>27.04</v>
       </c>
     </row>
-    <row r="115" spans="1:10">
+    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A115" s="3">
         <v>38813</v>
       </c>
@@ -5006,7 +5059,7 @@
         <v>77.36</v>
       </c>
     </row>
-    <row r="116" spans="1:10">
+    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A116" s="3">
         <v>38813</v>
       </c>
@@ -5038,7 +5091,7 @@
         <v>110.15</v>
       </c>
     </row>
-    <row r="117" spans="1:10">
+    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A117" s="3">
         <v>38813</v>
       </c>
@@ -5070,7 +5123,7 @@
         <v>62.43</v>
       </c>
     </row>
-    <row r="118" spans="1:10">
+    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A118" s="3">
         <v>38813</v>
       </c>
@@ -5102,7 +5155,7 @@
         <v>42.59</v>
       </c>
     </row>
-    <row r="119" spans="1:10">
+    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A119" s="3">
         <v>38814</v>
       </c>
@@ -5134,7 +5187,7 @@
         <v>112.57</v>
       </c>
     </row>
-    <row r="120" spans="1:10">
+    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A120" s="3">
         <v>38815</v>
       </c>
@@ -5166,7 +5219,7 @@
         <v>73.180000000000007</v>
       </c>
     </row>
-    <row r="121" spans="1:10">
+    <row r="121" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A121" s="3">
         <v>38815</v>
       </c>
@@ -5198,7 +5251,7 @@
         <v>87.4</v>
       </c>
     </row>
-    <row r="122" spans="1:10">
+    <row r="122" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A122" s="3">
         <v>38815</v>
       </c>
@@ -5230,7 +5283,7 @@
         <v>42.33</v>
       </c>
     </row>
-    <row r="123" spans="1:10">
+    <row r="123" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A123" s="3">
         <v>38815</v>
       </c>
@@ -5262,7 +5315,7 @@
         <v>70.319999999999993</v>
       </c>
     </row>
-    <row r="124" spans="1:10">
+    <row r="124" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A124" s="3">
         <v>38816</v>
       </c>
@@ -5294,7 +5347,7 @@
         <v>46.45</v>
       </c>
     </row>
-    <row r="125" spans="1:10">
+    <row r="125" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A125" s="3">
         <v>38817</v>
       </c>
@@ -5326,7 +5379,7 @@
         <v>48.12</v>
       </c>
     </row>
-    <row r="126" spans="1:10">
+    <row r="126" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A126" s="3">
         <v>38817</v>
       </c>
@@ -5358,7 +5411,7 @@
         <v>32.43</v>
       </c>
     </row>
-    <row r="127" spans="1:10">
+    <row r="127" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A127" s="3">
         <v>38817</v>
       </c>
@@ -5390,7 +5443,7 @@
         <v>65.349999999999994</v>
       </c>
     </row>
-    <row r="128" spans="1:10">
+    <row r="128" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A128" s="3">
         <v>38818</v>
       </c>
@@ -5422,7 +5475,7 @@
         <v>53.07</v>
       </c>
     </row>
-    <row r="129" spans="1:10">
+    <row r="129" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A129" s="3">
         <v>38818</v>
       </c>
@@ -5454,7 +5507,7 @@
         <v>31.98</v>
       </c>
     </row>
-    <row r="130" spans="1:10">
+    <row r="130" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A130" s="3">
         <v>38818</v>
       </c>
@@ -5486,7 +5539,7 @@
         <v>60.74</v>
       </c>
     </row>
-    <row r="131" spans="1:10">
+    <row r="131" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A131" s="3">
         <v>38818</v>
       </c>
@@ -5518,7 +5571,7 @@
         <v>56.09</v>
       </c>
     </row>
-    <row r="132" spans="1:10">
+    <row r="132" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A132" s="3">
         <v>38818</v>
       </c>
@@ -5550,7 +5603,7 @@
         <v>49.84</v>
       </c>
     </row>
-    <row r="133" spans="1:10">
+    <row r="133" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A133" s="3">
         <v>38818</v>
       </c>
@@ -5582,7 +5635,7 @@
         <v>39.04</v>
       </c>
     </row>
-    <row r="134" spans="1:10">
+    <row r="134" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A134" s="3">
         <v>38818</v>
       </c>
@@ -5614,7 +5667,7 @@
         <v>337.44</v>
       </c>
     </row>
-    <row r="135" spans="1:10">
+    <row r="135" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A135" s="3">
         <v>38819</v>
       </c>
@@ -5646,7 +5699,7 @@
         <v>89.43</v>
       </c>
     </row>
-    <row r="136" spans="1:10">
+    <row r="136" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A136" s="3">
         <v>38819</v>
       </c>
@@ -5678,7 +5731,7 @@
         <v>47.6</v>
       </c>
     </row>
-    <row r="137" spans="1:10">
+    <row r="137" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A137" s="3">
         <v>38819</v>
       </c>
@@ -5710,7 +5763,7 @@
         <v>27.99</v>
       </c>
     </row>
-    <row r="138" spans="1:10">
+    <row r="138" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A138" s="3">
         <v>38820</v>
       </c>
@@ -5742,7 +5795,7 @@
         <v>50.27</v>
       </c>
     </row>
-    <row r="139" spans="1:10">
+    <row r="139" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A139" s="3">
         <v>38820</v>
       </c>
@@ -5774,7 +5827,7 @@
         <v>81.56</v>
       </c>
     </row>
-    <row r="140" spans="1:10">
+    <row r="140" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A140" s="3">
         <v>38820</v>
       </c>
@@ -5806,7 +5859,7 @@
         <v>57.88</v>
       </c>
     </row>
-    <row r="141" spans="1:10">
+    <row r="141" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A141" s="3">
         <v>38821</v>
       </c>
@@ -5838,7 +5891,7 @@
         <v>61.84</v>
       </c>
     </row>
-    <row r="142" spans="1:10">
+    <row r="142" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A142" s="3">
         <v>38821</v>
       </c>
@@ -5870,7 +5923,7 @@
         <v>28.98</v>
       </c>
     </row>
-    <row r="143" spans="1:10">
+    <row r="143" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A143" s="3">
         <v>38821</v>
       </c>
@@ -5902,7 +5955,7 @@
         <v>55.4</v>
       </c>
     </row>
-    <row r="144" spans="1:10">
+    <row r="144" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A144" s="3">
         <v>38822</v>
       </c>
@@ -5934,7 +5987,7 @@
         <v>52.81</v>
       </c>
     </row>
-    <row r="145" spans="1:10">
+    <row r="145" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A145" s="3">
         <v>38822</v>
       </c>
@@ -5966,7 +6019,7 @@
         <v>41.29</v>
       </c>
     </row>
-    <row r="146" spans="1:10">
+    <row r="146" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A146" s="3">
         <v>38822</v>
       </c>
@@ -5998,7 +6051,7 @@
         <v>37.119999999999997</v>
       </c>
     </row>
-    <row r="147" spans="1:10">
+    <row r="147" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A147" s="3">
         <v>38823</v>
       </c>
@@ -6030,7 +6083,7 @@
         <v>32.299999999999997</v>
       </c>
     </row>
-    <row r="148" spans="1:10">
+    <row r="148" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A148" s="3">
         <v>38823</v>
       </c>
@@ -6062,7 +6115,7 @@
         <v>56.24</v>
       </c>
     </row>
-    <row r="149" spans="1:10">
+    <row r="149" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A149" s="3">
         <v>38823</v>
       </c>
@@ -6094,7 +6147,7 @@
         <v>35.14</v>
       </c>
     </row>
-    <row r="150" spans="1:10">
+    <row r="150" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A150" s="3">
         <v>38824</v>
       </c>
@@ -6126,7 +6179,7 @@
         <v>87.53</v>
       </c>
     </row>
-    <row r="151" spans="1:10">
+    <row r="151" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A151" s="3">
         <v>38824</v>
       </c>
@@ -6158,7 +6211,7 @@
         <v>183.78</v>
       </c>
     </row>
-    <row r="152" spans="1:10">
+    <row r="152" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A152" s="3">
         <v>38824</v>
       </c>
@@ -6190,7 +6243,7 @@
         <v>46.2</v>
       </c>
     </row>
-    <row r="153" spans="1:10">
+    <row r="153" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A153" s="3">
         <v>38824</v>
       </c>
@@ -6222,7 +6275,7 @@
         <v>160.99</v>
       </c>
     </row>
-    <row r="154" spans="1:10">
+    <row r="154" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A154" s="3">
         <v>38825</v>
       </c>
@@ -6254,7 +6307,7 @@
         <v>77.14</v>
       </c>
     </row>
-    <row r="155" spans="1:10">
+    <row r="155" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A155" s="3">
         <v>38825</v>
       </c>
@@ -6286,7 +6339,7 @@
         <v>96.4</v>
       </c>
     </row>
-    <row r="156" spans="1:10">
+    <row r="156" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A156" s="3">
         <v>38825</v>
       </c>
@@ -6318,7 +6371,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="157" spans="1:10">
+    <row r="157" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A157" s="3">
         <v>38826</v>
       </c>
@@ -6350,7 +6403,7 @@
         <v>74.27</v>
       </c>
     </row>
-    <row r="158" spans="1:10">
+    <row r="158" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A158" s="3">
         <v>38826</v>
       </c>
@@ -6382,7 +6435,7 @@
         <v>45.35</v>
       </c>
     </row>
-    <row r="159" spans="1:10">
+    <row r="159" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A159" s="3">
         <v>38827</v>
       </c>
@@ -6414,7 +6467,7 @@
         <v>105.74</v>
       </c>
     </row>
-    <row r="160" spans="1:10">
+    <row r="160" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A160" s="3">
         <v>38827</v>
       </c>
@@ -6446,7 +6499,7 @@
         <v>244.3</v>
       </c>
     </row>
-    <row r="161" spans="1:10">
+    <row r="161" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A161" s="3">
         <v>38827</v>
       </c>
@@ -6478,7 +6531,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="162" spans="1:10">
+    <row r="162" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A162" s="3">
         <v>38827</v>
       </c>
@@ -6510,7 +6563,7 @@
         <v>265.16000000000003</v>
       </c>
     </row>
-    <row r="163" spans="1:10">
+    <row r="163" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A163" s="3">
         <v>38827</v>
       </c>
@@ -6542,7 +6595,7 @@
         <v>206.33</v>
       </c>
     </row>
-    <row r="164" spans="1:10">
+    <row r="164" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A164" s="3">
         <v>38827</v>
       </c>
@@ -6574,7 +6627,7 @@
         <v>56.84</v>
       </c>
     </row>
-    <row r="165" spans="1:10">
+    <row r="165" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A165" s="3">
         <v>38828</v>
       </c>
@@ -6606,7 +6659,7 @@
         <v>121.06</v>
       </c>
     </row>
-    <row r="166" spans="1:10">
+    <row r="166" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A166" s="3">
         <v>38828</v>
       </c>
@@ -6638,7 +6691,7 @@
         <v>109.83</v>
       </c>
     </row>
-    <row r="167" spans="1:10">
+    <row r="167" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A167" s="3">
         <v>38829</v>
       </c>
@@ -6670,7 +6723,7 @@
         <v>81.75</v>
       </c>
     </row>
-    <row r="168" spans="1:10">
+    <row r="168" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A168" s="3">
         <v>38829</v>
       </c>
@@ -6702,7 +6755,7 @@
         <v>245.12</v>
       </c>
     </row>
-    <row r="169" spans="1:10">
+    <row r="169" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A169" s="3">
         <v>38829</v>
       </c>
@@ -6734,7 +6787,7 @@
         <v>78.569999999999993</v>
       </c>
     </row>
-    <row r="170" spans="1:10">
+    <row r="170" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A170" s="3">
         <v>38830</v>
       </c>
@@ -6766,7 +6819,7 @@
         <v>206.62</v>
       </c>
     </row>
-    <row r="171" spans="1:10">
+    <row r="171" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A171" s="3">
         <v>38830</v>
       </c>
@@ -6798,7 +6851,7 @@
         <v>61.57</v>
       </c>
     </row>
-    <row r="172" spans="1:10">
+    <row r="172" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A172" s="3">
         <v>38830</v>
       </c>
@@ -6830,7 +6883,7 @@
         <v>109.78</v>
       </c>
     </row>
-    <row r="173" spans="1:10">
+    <row r="173" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A173" s="3">
         <v>38831</v>
       </c>
@@ -6862,7 +6915,7 @@
         <v>164.77</v>
       </c>
     </row>
-    <row r="174" spans="1:10">
+    <row r="174" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A174" s="3">
         <v>38831</v>
       </c>
@@ -6894,7 +6947,7 @@
         <v>42.07</v>
       </c>
     </row>
-    <row r="175" spans="1:10">
+    <row r="175" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A175" s="3">
         <v>38831</v>
       </c>
@@ -6926,7 +6979,7 @@
         <v>39.979999999999997</v>
       </c>
     </row>
-    <row r="176" spans="1:10">
+    <row r="176" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A176" s="3">
         <v>38831</v>
       </c>
@@ -6958,7 +7011,7 @@
         <v>63.8</v>
       </c>
     </row>
-    <row r="177" spans="1:10">
+    <row r="177" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A177" s="3">
         <v>38832</v>
       </c>
@@ -6990,7 +7043,7 @@
         <v>90.86</v>
       </c>
     </row>
-    <row r="178" spans="1:10">
+    <row r="178" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A178" s="3">
         <v>38832</v>
       </c>
@@ -7022,7 +7075,7 @@
         <v>108.53</v>
       </c>
     </row>
-    <row r="179" spans="1:10">
+    <row r="179" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A179" s="3">
         <v>38832</v>
       </c>
@@ -7054,7 +7107,7 @@
         <v>54.14</v>
       </c>
     </row>
-    <row r="180" spans="1:10">
+    <row r="180" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A180" s="3">
         <v>38832</v>
       </c>
@@ -7086,7 +7139,7 @@
         <v>98.16</v>
       </c>
     </row>
-    <row r="181" spans="1:10">
+    <row r="181" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A181" s="3">
         <v>38832</v>
       </c>
@@ -7118,7 +7171,7 @@
         <v>72.8</v>
       </c>
     </row>
-    <row r="182" spans="1:10">
+    <row r="182" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A182" s="3">
         <v>38832</v>
       </c>
@@ -7150,7 +7203,7 @@
         <v>102.31</v>
       </c>
     </row>
-    <row r="183" spans="1:10">
+    <row r="183" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A183" s="3">
         <v>38832</v>
       </c>
@@ -7182,7 +7235,7 @@
         <v>89.07</v>
       </c>
     </row>
-    <row r="184" spans="1:10">
+    <row r="184" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A184" s="3">
         <v>38833</v>
       </c>
@@ -7214,7 +7267,7 @@
         <v>72.05</v>
       </c>
     </row>
-    <row r="185" spans="1:10">
+    <row r="185" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A185" s="3">
         <v>38833</v>
       </c>
@@ -7246,7 +7299,7 @@
         <v>60.23</v>
       </c>
     </row>
-    <row r="186" spans="1:10">
+    <row r="186" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A186" s="3">
         <v>38833</v>
       </c>
@@ -7278,7 +7331,7 @@
         <v>261.41000000000003</v>
       </c>
     </row>
-    <row r="187" spans="1:10">
+    <row r="187" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A187" s="3">
         <v>38834</v>
       </c>
@@ -7310,7 +7363,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="188" spans="1:10">
+    <row r="188" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A188" s="3">
         <v>38835</v>
       </c>
@@ -7342,7 +7395,7 @@
         <v>70.47</v>
       </c>
     </row>
-    <row r="189" spans="1:10">
+    <row r="189" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A189" s="3">
         <v>38836</v>
       </c>
@@ -7374,7 +7427,7 @@
         <v>112.28</v>
       </c>
     </row>
-    <row r="190" spans="1:10">
+    <row r="190" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A190" s="3">
         <v>38836</v>
       </c>
@@ -7406,7 +7459,7 @@
         <v>100.11</v>
       </c>
     </row>
-    <row r="191" spans="1:10">
+    <row r="191" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A191" s="3">
         <v>38837</v>
       </c>
@@ -7438,7 +7491,7 @@
         <v>343.29</v>
       </c>
     </row>
-    <row r="192" spans="1:10">
+    <row r="192" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A192" s="3">
         <v>38838</v>
       </c>
@@ -7470,7 +7523,7 @@
         <v>81.75</v>
       </c>
     </row>
-    <row r="193" spans="1:10">
+    <row r="193" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A193" s="3">
         <v>38838</v>
       </c>
@@ -7502,7 +7555,7 @@
         <v>36.200000000000003</v>
       </c>
     </row>
-    <row r="194" spans="1:10">
+    <row r="194" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A194" s="3">
         <v>38839</v>
       </c>
@@ -7534,7 +7587,7 @@
         <v>24.02</v>
       </c>
     </row>
-    <row r="195" spans="1:10">
+    <row r="195" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A195" s="3">
         <v>38839</v>
       </c>
@@ -7566,7 +7619,7 @@
         <v>92.3</v>
       </c>
     </row>
-    <row r="196" spans="1:10">
+    <row r="196" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A196" s="3">
         <v>38839</v>
       </c>
@@ -7598,7 +7651,7 @@
         <v>47.7</v>
       </c>
     </row>
-    <row r="197" spans="1:10">
+    <row r="197" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A197" s="3">
         <v>38839</v>
       </c>
@@ -7630,7 +7683,7 @@
         <v>74.930000000000007</v>
       </c>
     </row>
-    <row r="198" spans="1:10">
+    <row r="198" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A198" s="3">
         <v>38839</v>
       </c>
@@ -7662,7 +7715,7 @@
         <v>87.1</v>
       </c>
     </row>
-    <row r="199" spans="1:10">
+    <row r="199" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A199" s="3">
         <v>38839</v>
       </c>
@@ -7694,7 +7747,7 @@
         <v>54.71</v>
       </c>
     </row>
-    <row r="200" spans="1:10">
+    <row r="200" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A200" s="3">
         <v>38839</v>
       </c>
@@ -7726,7 +7779,7 @@
         <v>78.41</v>
       </c>
     </row>
-    <row r="201" spans="1:10">
+    <row r="201" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A201" s="3">
         <v>38839</v>
       </c>
@@ -7758,7 +7811,7 @@
         <v>34.31</v>
       </c>
     </row>
-    <row r="202" spans="1:10">
+    <row r="202" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A202" s="3">
         <v>38839</v>
       </c>
@@ -7790,7 +7843,7 @@
         <v>69.680000000000007</v>
       </c>
     </row>
-    <row r="203" spans="1:10">
+    <row r="203" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A203" s="3">
         <v>38839</v>
       </c>
@@ -7822,7 +7875,7 @@
         <v>66.83</v>
       </c>
     </row>
-    <row r="204" spans="1:10">
+    <row r="204" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A204" s="3">
         <v>38840</v>
       </c>
@@ -7854,7 +7907,7 @@
         <v>65.92</v>
       </c>
     </row>
-    <row r="205" spans="1:10">
+    <row r="205" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A205" s="3">
         <v>38840</v>
       </c>
@@ -7886,7 +7939,7 @@
         <v>89.98</v>
       </c>
     </row>
-    <row r="206" spans="1:10">
+    <row r="206" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A206" s="3">
         <v>38841</v>
       </c>
@@ -7918,7 +7971,7 @@
         <v>75.69</v>
       </c>
     </row>
-    <row r="207" spans="1:10">
+    <row r="207" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A207" s="3">
         <v>38841</v>
       </c>
@@ -7950,7 +8003,7 @@
         <v>101.42</v>
       </c>
     </row>
-    <row r="208" spans="1:10">
+    <row r="208" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A208" s="3">
         <v>38841</v>
       </c>
@@ -7982,7 +8035,7 @@
         <v>99.33</v>
       </c>
     </row>
-    <row r="209" spans="1:10">
+    <row r="209" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A209" s="3">
         <v>38841</v>
       </c>
@@ -8014,7 +8067,7 @@
         <v>183.62</v>
       </c>
     </row>
-    <row r="210" spans="1:10">
+    <row r="210" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A210" s="3">
         <v>38841</v>
       </c>
@@ -8046,7 +8099,7 @@
         <v>83.41</v>
       </c>
     </row>
-    <row r="211" spans="1:10">
+    <row r="211" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A211" s="3">
         <v>38841</v>
       </c>
@@ -8078,7 +8131,7 @@
         <v>60.67</v>
       </c>
     </row>
-    <row r="212" spans="1:10">
+    <row r="212" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A212" s="3">
         <v>38842</v>
       </c>
@@ -8110,7 +8163,7 @@
         <v>204.41</v>
       </c>
     </row>
-    <row r="213" spans="1:10">
+    <row r="213" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A213" s="3">
         <v>38842</v>
       </c>
@@ -8142,7 +8195,7 @@
         <v>73.39</v>
       </c>
     </row>
-    <row r="214" spans="1:10">
+    <row r="214" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A214" s="3">
         <v>38842</v>
       </c>
@@ -8174,7 +8227,7 @@
         <v>226.18</v>
       </c>
     </row>
-    <row r="215" spans="1:10">
+    <row r="215" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A215" s="3">
         <v>38842</v>
       </c>
@@ -8206,7 +8259,7 @@
         <v>140.72999999999999</v>
       </c>
     </row>
-    <row r="216" spans="1:10">
+    <row r="216" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A216" s="3">
         <v>38843</v>
       </c>
@@ -8238,7 +8291,7 @@
         <v>66.23</v>
       </c>
     </row>
-    <row r="217" spans="1:10">
+    <row r="217" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A217" s="3">
         <v>38843</v>
       </c>
@@ -8270,7 +8323,7 @@
         <v>79.16</v>
       </c>
     </row>
-    <row r="218" spans="1:10">
+    <row r="218" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A218" s="3">
         <v>38844</v>
       </c>
@@ -8302,7 +8355,7 @@
         <v>260.67</v>
       </c>
     </row>
-    <row r="219" spans="1:10">
+    <row r="219" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A219" s="3">
         <v>38844</v>
       </c>
@@ -8334,7 +8387,7 @@
         <v>46.71</v>
       </c>
     </row>
-    <row r="220" spans="1:10">
+    <row r="220" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A220" s="3">
         <v>38845</v>
       </c>
@@ -8366,7 +8419,7 @@
         <v>74.17</v>
       </c>
     </row>
-    <row r="221" spans="1:10">
+    <row r="221" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A221" s="3">
         <v>38845</v>
       </c>
@@ -8398,7 +8451,7 @@
         <v>112.54</v>
       </c>
     </row>
-    <row r="222" spans="1:10">
+    <row r="222" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A222" s="3">
         <v>38846</v>
       </c>
@@ -8430,7 +8483,7 @@
         <v>121.01</v>
       </c>
     </row>
-    <row r="223" spans="1:10">
+    <row r="223" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A223" s="3">
         <v>38846</v>
       </c>
@@ -8462,7 +8515,7 @@
         <v>98.74</v>
       </c>
     </row>
-    <row r="224" spans="1:10">
+    <row r="224" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A224" s="3">
         <v>38846</v>
       </c>
@@ -8494,7 +8547,7 @@
         <v>101.05</v>
       </c>
     </row>
-    <row r="225" spans="1:10">
+    <row r="225" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A225" s="3">
         <v>38846</v>
       </c>
@@ -8526,7 +8579,7 @@
         <v>203.01</v>
       </c>
     </row>
-    <row r="226" spans="1:10">
+    <row r="226" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A226" s="3">
         <v>38847</v>
       </c>
@@ -8558,7 +8611,7 @@
         <v>59.07</v>
       </c>
     </row>
-    <row r="227" spans="1:10">
+    <row r="227" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A227" s="3">
         <v>38848</v>
       </c>
@@ -8590,7 +8643,7 @@
         <v>52.68</v>
       </c>
     </row>
-    <row r="228" spans="1:10">
+    <row r="228" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A228" s="3">
         <v>38848</v>
       </c>
@@ -8622,7 +8675,7 @@
         <v>67.39</v>
       </c>
     </row>
-    <row r="229" spans="1:10">
+    <row r="229" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A229" s="3">
         <v>38848</v>
       </c>
@@ -8654,7 +8707,7 @@
         <v>85.29</v>
       </c>
     </row>
-    <row r="230" spans="1:10">
+    <row r="230" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A230" s="3">
         <v>38848</v>
       </c>
@@ -8686,7 +8739,7 @@
         <v>94.55</v>
       </c>
     </row>
-    <row r="231" spans="1:10">
+    <row r="231" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A231" s="3">
         <v>38848</v>
       </c>
@@ -8718,7 +8771,7 @@
         <v>91.86</v>
       </c>
     </row>
-    <row r="232" spans="1:10">
+    <row r="232" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A232" s="3">
         <v>38848</v>
       </c>
@@ -8750,7 +8803,7 @@
         <v>176.94</v>
       </c>
     </row>
-    <row r="233" spans="1:10">
+    <row r="233" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A233" s="3">
         <v>38848</v>
       </c>
@@ -8782,7 +8835,7 @@
         <v>56.17</v>
       </c>
     </row>
-    <row r="234" spans="1:10">
+    <row r="234" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A234" s="3">
         <v>38849</v>
       </c>
@@ -8814,7 +8867,7 @@
         <v>123.62</v>
       </c>
     </row>
-    <row r="235" spans="1:10">
+    <row r="235" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A235" s="3">
         <v>38849</v>
       </c>
@@ -8846,7 +8899,7 @@
         <v>36.130000000000003</v>
       </c>
     </row>
-    <row r="236" spans="1:10">
+    <row r="236" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A236" s="3">
         <v>38849</v>
       </c>
@@ -8878,7 +8931,7 @@
         <v>259.24</v>
       </c>
     </row>
-    <row r="237" spans="1:10">
+    <row r="237" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A237" s="3">
         <v>38849</v>
       </c>
@@ -8910,7 +8963,7 @@
         <v>81.23</v>
       </c>
     </row>
-    <row r="238" spans="1:10">
+    <row r="238" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A238" s="3">
         <v>38850</v>
       </c>
@@ -8942,7 +8995,7 @@
         <v>170.73</v>
       </c>
     </row>
-    <row r="239" spans="1:10">
+    <row r="239" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A239" s="3">
         <v>38850</v>
       </c>
@@ -8974,7 +9027,7 @@
         <v>156.78</v>
       </c>
     </row>
-    <row r="240" spans="1:10">
+    <row r="240" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A240" s="3">
         <v>38850</v>
       </c>
@@ -9006,7 +9059,7 @@
         <v>276.64999999999998</v>
       </c>
     </row>
-    <row r="241" spans="1:10">
+    <row r="241" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A241" s="3">
         <v>38850</v>
       </c>
@@ -9038,7 +9091,7 @@
         <v>54.03</v>
       </c>
     </row>
-    <row r="242" spans="1:10">
+    <row r="242" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A242" s="3">
         <v>38851</v>
       </c>
@@ -9070,7 +9123,7 @@
         <v>79.489999999999995</v>
       </c>
     </row>
-    <row r="243" spans="1:10">
+    <row r="243" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A243" s="3">
         <v>38851</v>
       </c>
@@ -9102,7 +9155,7 @@
         <v>61.35</v>
       </c>
     </row>
-    <row r="244" spans="1:10">
+    <row r="244" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A244" s="3">
         <v>38851</v>
       </c>
@@ -9134,7 +9187,7 @@
         <v>62.6</v>
       </c>
     </row>
-    <row r="245" spans="1:10">
+    <row r="245" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A245" s="3">
         <v>38852</v>
       </c>
@@ -9166,7 +9219,7 @@
         <v>88.3</v>
       </c>
     </row>
-    <row r="246" spans="1:10">
+    <row r="246" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A246" s="3">
         <v>38852</v>
       </c>
@@ -9198,7 +9251,7 @@
         <v>232.77</v>
       </c>
     </row>
-    <row r="247" spans="1:10">
+    <row r="247" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A247" s="3">
         <v>38852</v>
       </c>
@@ -9230,7 +9283,7 @@
         <v>154.80000000000001</v>
       </c>
     </row>
-    <row r="248" spans="1:10">
+    <row r="248" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A248" s="3">
         <v>38852</v>
       </c>
@@ -9262,7 +9315,7 @@
         <v>93.42</v>
       </c>
     </row>
-    <row r="249" spans="1:10">
+    <row r="249" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A249" s="3">
         <v>38852</v>
       </c>
@@ -9294,7 +9347,7 @@
         <v>61.53</v>
       </c>
     </row>
-    <row r="250" spans="1:10">
+    <row r="250" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A250" s="3">
         <v>38852</v>
       </c>
@@ -9326,7 +9379,7 @@
         <v>77.849999999999994</v>
       </c>
     </row>
-    <row r="251" spans="1:10">
+    <row r="251" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A251" s="3">
         <v>38852</v>
       </c>
@@ -9358,7 +9411,7 @@
         <v>159.16999999999999</v>
       </c>
     </row>
-    <row r="252" spans="1:10">
+    <row r="252" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A252" s="3">
         <v>38852</v>
       </c>
@@ -9390,7 +9443,7 @@
         <v>70.06</v>
       </c>
     </row>
-    <row r="253" spans="1:10">
+    <row r="253" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A253" s="3">
         <v>38852</v>
       </c>
@@ -9422,7 +9475,7 @@
         <v>42.32</v>
       </c>
     </row>
-    <row r="254" spans="1:10">
+    <row r="254" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A254" s="3">
         <v>38852</v>
       </c>
@@ -9454,7 +9507,7 @@
         <v>123.59</v>
       </c>
     </row>
-    <row r="255" spans="1:10">
+    <row r="255" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A255" s="3">
         <v>38853</v>
       </c>
@@ -9486,7 +9539,7 @@
         <v>130.65</v>
       </c>
     </row>
-    <row r="256" spans="1:10">
+    <row r="256" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A256" s="3">
         <v>38854</v>
       </c>
@@ -9518,7 +9571,7 @@
         <v>49.62</v>
       </c>
     </row>
-    <row r="257" spans="1:10">
+    <row r="257" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A257" s="3">
         <v>38854</v>
       </c>
@@ -9550,7 +9603,7 @@
         <v>74.180000000000007</v>
       </c>
     </row>
-    <row r="258" spans="1:10">
+    <row r="258" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A258" s="3">
         <v>38854</v>
       </c>
@@ -9582,7 +9635,7 @@
         <v>137.61000000000001</v>
       </c>
     </row>
-    <row r="259" spans="1:10">
+    <row r="259" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A259" s="3">
         <v>38854</v>
       </c>
@@ -9614,7 +9667,7 @@
         <v>54.33</v>
       </c>
     </row>
-    <row r="260" spans="1:10">
+    <row r="260" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A260" s="3">
         <v>38855</v>
       </c>
@@ -9646,7 +9699,7 @@
         <v>87.83</v>
       </c>
     </row>
-    <row r="261" spans="1:10">
+    <row r="261" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A261" s="3">
         <v>38855</v>
       </c>
@@ -9678,7 +9731,7 @@
         <v>66.33</v>
       </c>
     </row>
-    <row r="262" spans="1:10">
+    <row r="262" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A262" s="3">
         <v>38855</v>
       </c>
@@ -9710,7 +9763,7 @@
         <v>68.260000000000005</v>
       </c>
     </row>
-    <row r="263" spans="1:10">
+    <row r="263" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A263" s="3">
         <v>38855</v>
       </c>
@@ -9742,7 +9795,7 @@
         <v>232.22</v>
       </c>
     </row>
-    <row r="264" spans="1:10">
+    <row r="264" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A264" s="3">
         <v>38855</v>
       </c>
@@ -9774,7 +9827,7 @@
         <v>182.62</v>
       </c>
     </row>
-    <row r="265" spans="1:10">
+    <row r="265" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A265" s="3">
         <v>38855</v>
       </c>
@@ -9806,7 +9859,7 @@
         <v>75.89</v>
       </c>
     </row>
-    <row r="266" spans="1:10">
+    <row r="266" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A266" s="3">
         <v>38856</v>
       </c>
@@ -9838,7 +9891,7 @@
         <v>55.55</v>
       </c>
     </row>
-    <row r="267" spans="1:10">
+    <row r="267" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A267" s="3">
         <v>38857</v>
       </c>
@@ -9870,7 +9923,7 @@
         <v>82.63</v>
       </c>
     </row>
-    <row r="268" spans="1:10">
+    <row r="268" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A268" s="3">
         <v>38857</v>
       </c>
@@ -9902,7 +9955,7 @@
         <v>58.37</v>
       </c>
     </row>
-    <row r="269" spans="1:10">
+    <row r="269" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A269" s="3">
         <v>38857</v>
       </c>
@@ -9934,7 +9987,7 @@
         <v>175.8</v>
       </c>
     </row>
-    <row r="270" spans="1:10">
+    <row r="270" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A270" s="3">
         <v>38858</v>
       </c>
@@ -9966,7 +10019,7 @@
         <v>107.36</v>
       </c>
     </row>
-    <row r="271" spans="1:10">
+    <row r="271" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A271" s="3">
         <v>38858</v>
       </c>
@@ -9998,7 +10051,7 @@
         <v>258.11</v>
       </c>
     </row>
-    <row r="272" spans="1:10">
+    <row r="272" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A272" s="3">
         <v>38858</v>
       </c>
@@ -10030,7 +10083,7 @@
         <v>289.27</v>
       </c>
     </row>
-    <row r="273" spans="1:10">
+    <row r="273" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A273" s="3">
         <v>38859</v>
       </c>
@@ -10062,7 +10115,7 @@
         <v>201.43</v>
       </c>
     </row>
-    <row r="274" spans="1:10">
+    <row r="274" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A274" s="3">
         <v>38859</v>
       </c>
@@ -10094,7 +10147,7 @@
         <v>161.16999999999999</v>
       </c>
     </row>
-    <row r="275" spans="1:10">
+    <row r="275" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A275" s="3">
         <v>38859</v>
       </c>
@@ -10126,7 +10179,7 @@
         <v>53.91</v>
       </c>
     </row>
-    <row r="276" spans="1:10">
+    <row r="276" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A276" s="3">
         <v>38859</v>
       </c>
@@ -10158,7 +10211,7 @@
         <v>55.28</v>
       </c>
     </row>
-    <row r="277" spans="1:10">
+    <row r="277" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A277" s="3">
         <v>38860</v>
       </c>
@@ -10190,7 +10243,7 @@
         <v>84.06</v>
       </c>
     </row>
-    <row r="278" spans="1:10">
+    <row r="278" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A278" s="3">
         <v>38860</v>
       </c>
@@ -10222,7 +10275,7 @@
         <v>357.16</v>
       </c>
     </row>
-    <row r="279" spans="1:10">
+    <row r="279" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A279" s="3">
         <v>38861</v>
       </c>
@@ -10254,7 +10307,7 @@
         <v>170.51</v>
       </c>
     </row>
-    <row r="280" spans="1:10">
+    <row r="280" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A280" s="3">
         <v>38861</v>
       </c>
@@ -10286,7 +10339,7 @@
         <v>57.19</v>
       </c>
     </row>
-    <row r="281" spans="1:10">
+    <row r="281" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A281" s="3">
         <v>38862</v>
       </c>
@@ -10318,7 +10371,7 @@
         <v>120.36</v>
       </c>
     </row>
-    <row r="282" spans="1:10">
+    <row r="282" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A282" s="3">
         <v>38862</v>
       </c>
@@ -10350,7 +10403,7 @@
         <v>43.32</v>
       </c>
     </row>
-    <row r="283" spans="1:10">
+    <row r="283" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A283" s="3">
         <v>38863</v>
       </c>
@@ -10382,7 +10435,7 @@
         <v>224.18</v>
       </c>
     </row>
-    <row r="284" spans="1:10">
+    <row r="284" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A284" s="3">
         <v>38863</v>
       </c>
@@ -10414,7 +10467,7 @@
         <v>109.08</v>
       </c>
     </row>
-    <row r="285" spans="1:10">
+    <row r="285" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A285" s="3">
         <v>38863</v>
       </c>
@@ -10446,7 +10499,7 @@
         <v>62.3</v>
       </c>
     </row>
-    <row r="286" spans="1:10">
+    <row r="286" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A286" s="3">
         <v>38863</v>
       </c>
@@ -10478,7 +10531,7 @@
         <v>87.72</v>
       </c>
     </row>
-    <row r="287" spans="1:10">
+    <row r="287" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A287" s="3">
         <v>38864</v>
       </c>
@@ -10510,7 +10563,7 @@
         <v>63.75</v>
       </c>
     </row>
-    <row r="288" spans="1:10">
+    <row r="288" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A288" s="3">
         <v>38864</v>
       </c>
@@ -10542,7 +10595,7 @@
         <v>169.45</v>
       </c>
     </row>
-    <row r="289" spans="1:10">
+    <row r="289" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A289" s="3">
         <v>38864</v>
       </c>
@@ -10574,7 +10627,7 @@
         <v>65.77</v>
       </c>
     </row>
-    <row r="290" spans="1:10">
+    <row r="290" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A290" s="3">
         <v>38864</v>
       </c>
@@ -10606,7 +10659,7 @@
         <v>266.82</v>
       </c>
     </row>
-    <row r="291" spans="1:10">
+    <row r="291" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A291" s="3">
         <v>38864</v>
       </c>
@@ -10638,7 +10691,7 @@
         <v>51.37</v>
       </c>
     </row>
-    <row r="292" spans="1:10">
+    <row r="292" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A292" s="3">
         <v>38865</v>
       </c>
@@ -10670,7 +10723,7 @@
         <v>240.44</v>
       </c>
     </row>
-    <row r="293" spans="1:10">
+    <row r="293" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A293" s="3">
         <v>38865</v>
       </c>
@@ -10702,7 +10755,7 @@
         <v>92.71</v>
       </c>
     </row>
-    <row r="294" spans="1:10">
+    <row r="294" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A294" s="3">
         <v>38865</v>
       </c>
@@ -10734,7 +10787,7 @@
         <v>115.55</v>
       </c>
     </row>
-    <row r="295" spans="1:10">
+    <row r="295" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A295" s="3">
         <v>38865</v>
       </c>
@@ -10766,7 +10819,7 @@
         <v>119.68</v>
       </c>
     </row>
-    <row r="296" spans="1:10">
+    <row r="296" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A296" s="3">
         <v>38865</v>
       </c>
@@ -10798,7 +10851,7 @@
         <v>103.15</v>
       </c>
     </row>
-    <row r="297" spans="1:10">
+    <row r="297" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A297" s="3">
         <v>38865</v>
       </c>
@@ -10830,7 +10883,7 @@
         <v>67.72</v>
       </c>
     </row>
-    <row r="298" spans="1:10">
+    <row r="298" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A298" s="3">
         <v>38865</v>
       </c>
@@ -10862,7 +10915,7 @@
         <v>117.99</v>
       </c>
     </row>
-    <row r="299" spans="1:10">
+    <row r="299" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A299" s="3">
         <v>38865</v>
       </c>
@@ -10894,7 +10947,7 @@
         <v>54.22</v>
       </c>
     </row>
-    <row r="300" spans="1:10">
+    <row r="300" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A300" s="3">
         <v>38866</v>
       </c>
@@ -10926,7 +10979,7 @@
         <v>87.91</v>
       </c>
     </row>
-    <row r="301" spans="1:10">
+    <row r="301" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A301" s="3">
         <v>38866</v>
       </c>
@@ -10958,7 +11011,7 @@
         <v>56.32</v>
       </c>
     </row>
-    <row r="302" spans="1:10">
+    <row r="302" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A302" s="3">
         <v>38867</v>
       </c>
@@ -10990,7 +11043,7 @@
         <v>72.709999999999994</v>
       </c>
     </row>
-    <row r="303" spans="1:10">
+    <row r="303" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A303" s="3">
         <v>38867</v>
       </c>
@@ -11022,7 +11075,7 @@
         <v>138.41999999999999</v>
       </c>
     </row>
-    <row r="304" spans="1:10">
+    <row r="304" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A304" s="3">
         <v>38868</v>
       </c>
@@ -11054,7 +11107,7 @@
         <v>144.66</v>
       </c>
     </row>
-    <row r="305" spans="1:10">
+    <row r="305" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A305" s="3">
         <v>38868</v>
       </c>
@@ -11086,7 +11139,7 @@
         <v>78.709999999999994</v>
       </c>
     </row>
-    <row r="306" spans="1:10">
+    <row r="306" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A306" s="3">
         <v>38868</v>
       </c>
@@ -11118,7 +11171,7 @@
         <v>58.32</v>
       </c>
     </row>
-    <row r="307" spans="1:10">
+    <row r="307" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A307" s="3">
         <v>38868</v>
       </c>
@@ -11150,7 +11203,7 @@
         <v>96.46</v>
       </c>
     </row>
-    <row r="308" spans="1:10">
+    <row r="308" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A308" s="3">
         <v>38868</v>
       </c>
@@ -11182,7 +11235,7 @@
         <v>125.25</v>
       </c>
     </row>
-    <row r="309" spans="1:10">
+    <row r="309" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A309" s="3">
         <v>38869</v>
       </c>
@@ -11214,7 +11267,7 @@
         <v>90.09</v>
       </c>
     </row>
-    <row r="310" spans="1:10">
+    <row r="310" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A310" s="3">
         <v>38870</v>
       </c>
@@ -11246,7 +11299,7 @@
         <v>107.71</v>
       </c>
     </row>
-    <row r="311" spans="1:10">
+    <row r="311" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A311" s="3">
         <v>38870</v>
       </c>
@@ -11278,7 +11331,7 @@
         <v>93.82</v>
       </c>
     </row>
-    <row r="312" spans="1:10">
+    <row r="312" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A312" s="3">
         <v>38870</v>
       </c>
@@ -11310,7 +11363,7 @@
         <v>93.82</v>
       </c>
     </row>
-    <row r="313" spans="1:10">
+    <row r="313" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A313" s="3">
         <v>38871</v>
       </c>
@@ -11342,7 +11395,7 @@
         <v>58.05</v>
       </c>
     </row>
-    <row r="314" spans="1:10">
+    <row r="314" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A314" s="3">
         <v>38871</v>
       </c>
@@ -11374,7 +11427,7 @@
         <v>149.15</v>
       </c>
     </row>
-    <row r="315" spans="1:10">
+    <row r="315" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A315" s="3">
         <v>38871</v>
       </c>
@@ -11406,7 +11459,7 @@
         <v>129.21</v>
       </c>
     </row>
-    <row r="316" spans="1:10">
+    <row r="316" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A316" s="3">
         <v>38871</v>
       </c>
@@ -11438,7 +11491,7 @@
         <v>283.26</v>
       </c>
     </row>
-    <row r="317" spans="1:10">
+    <row r="317" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A317" s="3">
         <v>38872</v>
       </c>
@@ -11470,7 +11523,7 @@
         <v>87.44</v>
       </c>
     </row>
-    <row r="318" spans="1:10">
+    <row r="318" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A318" s="3">
         <v>38872</v>
       </c>
@@ -11502,7 +11555,7 @@
         <v>159.25</v>
       </c>
     </row>
-    <row r="319" spans="1:10">
+    <row r="319" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A319" s="3">
         <v>38872</v>
       </c>
@@ -11534,7 +11587,7 @@
         <v>74.650000000000006</v>
       </c>
     </row>
-    <row r="320" spans="1:10">
+    <row r="320" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A320" s="3">
         <v>38872</v>
       </c>
@@ -11566,7 +11619,7 @@
         <v>113.37</v>
       </c>
     </row>
-    <row r="321" spans="1:10">
+    <row r="321" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A321" s="3">
         <v>38873</v>
       </c>
@@ -11598,7 +11651,7 @@
         <v>75.930000000000007</v>
       </c>
     </row>
-    <row r="322" spans="1:10">
+    <row r="322" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A322" s="3">
         <v>38874</v>
       </c>
@@ -11630,7 +11683,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="323" spans="1:10">
+    <row r="323" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A323" s="3">
         <v>38874</v>
       </c>
@@ -11662,7 +11715,7 @@
         <v>155.26</v>
       </c>
     </row>
-    <row r="324" spans="1:10">
+    <row r="324" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A324" s="3">
         <v>38874</v>
       </c>
@@ -11694,7 +11747,7 @@
         <v>339.72</v>
       </c>
     </row>
-    <row r="325" spans="1:10">
+    <row r="325" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A325" s="3">
         <v>38874</v>
       </c>
@@ -11726,7 +11779,7 @@
         <v>190.18</v>
       </c>
     </row>
-    <row r="326" spans="1:10">
+    <row r="326" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A326" s="3">
         <v>38874</v>
       </c>
@@ -11758,7 +11811,7 @@
         <v>61.19</v>
       </c>
     </row>
-    <row r="327" spans="1:10">
+    <row r="327" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A327" s="3">
         <v>38874</v>
       </c>
@@ -11790,7 +11843,7 @@
         <v>90.51</v>
       </c>
     </row>
-    <row r="328" spans="1:10">
+    <row r="328" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A328" s="3">
         <v>38875</v>
       </c>
@@ -11822,7 +11875,7 @@
         <v>58.52</v>
       </c>
     </row>
-    <row r="329" spans="1:10">
+    <row r="329" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A329" s="3">
         <v>38875</v>
       </c>
@@ -11854,7 +11907,7 @@
         <v>67.23</v>
       </c>
     </row>
-    <row r="330" spans="1:10">
+    <row r="330" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A330" s="3">
         <v>38875</v>
       </c>
@@ -11886,7 +11939,7 @@
         <v>90.87</v>
       </c>
     </row>
-    <row r="331" spans="1:10">
+    <row r="331" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A331" s="3">
         <v>38875</v>
       </c>
@@ -11918,7 +11971,7 @@
         <v>76.92</v>
       </c>
     </row>
-    <row r="332" spans="1:10">
+    <row r="332" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A332" s="3">
         <v>38875</v>
       </c>
@@ -11950,7 +12003,7 @@
         <v>175.5</v>
       </c>
     </row>
-    <row r="333" spans="1:10">
+    <row r="333" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A333" s="3">
         <v>38876</v>
       </c>
@@ -11982,7 +12035,7 @@
         <v>249.78</v>
       </c>
     </row>
-    <row r="334" spans="1:10">
+    <row r="334" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A334" s="3">
         <v>38876</v>
       </c>
@@ -12014,7 +12067,7 @@
         <v>119.5</v>
       </c>
     </row>
-    <row r="335" spans="1:10">
+    <row r="335" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A335" s="3">
         <v>38876</v>
       </c>
@@ -12046,7 +12099,7 @@
         <v>166.1</v>
       </c>
     </row>
-    <row r="336" spans="1:10">
+    <row r="336" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A336" s="3">
         <v>38876</v>
       </c>
@@ -12078,7 +12131,7 @@
         <v>84.15</v>
       </c>
     </row>
-    <row r="337" spans="1:10">
+    <row r="337" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A337" s="3">
         <v>38877</v>
       </c>
@@ -12110,7 +12163,7 @@
         <v>76.55</v>
       </c>
     </row>
-    <row r="338" spans="1:10">
+    <row r="338" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A338" s="3">
         <v>38877</v>
       </c>
@@ -12142,7 +12195,7 @@
         <v>250.78</v>
       </c>
     </row>
-    <row r="339" spans="1:10">
+    <row r="339" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A339" s="3">
         <v>38877</v>
       </c>
@@ -12174,7 +12227,7 @@
         <v>116.94</v>
       </c>
     </row>
-    <row r="340" spans="1:10">
+    <row r="340" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A340" s="3">
         <v>38878</v>
       </c>
@@ -12206,7 +12259,7 @@
         <v>49.37</v>
       </c>
     </row>
-    <row r="341" spans="1:10">
+    <row r="341" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A341" s="3">
         <v>38878</v>
       </c>
@@ -12238,7 +12291,7 @@
         <v>135.97</v>
       </c>
     </row>
-    <row r="342" spans="1:10">
+    <row r="342" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A342" s="3">
         <v>38878</v>
       </c>
@@ -12270,7 +12323,7 @@
         <v>87.14</v>
       </c>
     </row>
-    <row r="343" spans="1:10">
+    <row r="343" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A343" s="3">
         <v>38878</v>
       </c>
@@ -12302,7 +12355,7 @@
         <v>58.55</v>
       </c>
     </row>
-    <row r="344" spans="1:10">
+    <row r="344" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A344" s="3">
         <v>38878</v>
       </c>
@@ -12334,7 +12387,7 @@
         <v>74.739999999999995</v>
       </c>
     </row>
-    <row r="345" spans="1:10">
+    <row r="345" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A345" s="3">
         <v>38879</v>
       </c>
@@ -12366,7 +12419,7 @@
         <v>117.48</v>
       </c>
     </row>
-    <row r="346" spans="1:10">
+    <row r="346" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A346" s="3">
         <v>38879</v>
       </c>
@@ -12398,7 +12451,7 @@
         <v>115.69</v>
       </c>
     </row>
-    <row r="347" spans="1:10">
+    <row r="347" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A347" s="3">
         <v>38879</v>
       </c>
@@ -12430,7 +12483,7 @@
         <v>143.78</v>
       </c>
     </row>
-    <row r="348" spans="1:10">
+    <row r="348" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A348" s="3">
         <v>38879</v>
       </c>
@@ -12462,7 +12515,7 @@
         <v>78.06</v>
       </c>
     </row>
-    <row r="349" spans="1:10">
+    <row r="349" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A349" s="3">
         <v>38879</v>
       </c>
@@ -12494,7 +12547,7 @@
         <v>89.45</v>
       </c>
     </row>
-    <row r="350" spans="1:10">
+    <row r="350" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A350" s="3">
         <v>38880</v>
       </c>
@@ -12526,7 +12579,7 @@
         <v>91.62</v>
       </c>
     </row>
-    <row r="351" spans="1:10">
+    <row r="351" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A351" s="3">
         <v>38881</v>
       </c>
@@ -12558,7 +12611,7 @@
         <v>113.4</v>
       </c>
     </row>
-    <row r="352" spans="1:10">
+    <row r="352" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A352" s="3">
         <v>38881</v>
       </c>
@@ -12590,7 +12643,7 @@
         <v>108.97</v>
       </c>
     </row>
-    <row r="353" spans="1:10">
+    <row r="353" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A353" s="3">
         <v>38882</v>
       </c>
@@ -12622,7 +12675,7 @@
         <v>100.13</v>
       </c>
     </row>
-    <row r="354" spans="1:10">
+    <row r="354" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A354" s="3">
         <v>38882</v>
       </c>
@@ -12654,7 +12707,7 @@
         <v>91.91</v>
       </c>
     </row>
-    <row r="355" spans="1:10">
+    <row r="355" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A355" s="3">
         <v>38883</v>
       </c>
@@ -12686,7 +12739,7 @@
         <v>100.02</v>
       </c>
     </row>
-    <row r="356" spans="1:10">
+    <row r="356" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A356" s="3">
         <v>38883</v>
       </c>
@@ -12718,7 +12771,7 @@
         <v>134.97999999999999</v>
       </c>
     </row>
-    <row r="357" spans="1:10">
+    <row r="357" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A357" s="3">
         <v>38883</v>
       </c>
@@ -12750,7 +12803,7 @@
         <v>109.45</v>
       </c>
     </row>
-    <row r="358" spans="1:10">
+    <row r="358" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A358" s="3">
         <v>38884</v>
       </c>
@@ -12782,7 +12835,7 @@
         <v>45.43</v>
       </c>
     </row>
-    <row r="359" spans="1:10">
+    <row r="359" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A359" s="3">
         <v>38885</v>
       </c>
@@ -12814,7 +12867,7 @@
         <v>88.76</v>
       </c>
     </row>
-    <row r="360" spans="1:10">
+    <row r="360" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A360" s="3">
         <v>38885</v>
       </c>
@@ -12846,7 +12899,7 @@
         <v>119.76</v>
       </c>
     </row>
-    <row r="361" spans="1:10">
+    <row r="361" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A361" s="3">
         <v>38885</v>
       </c>
@@ -12878,7 +12931,7 @@
         <v>100.7</v>
       </c>
     </row>
-    <row r="362" spans="1:10">
+    <row r="362" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A362" s="3">
         <v>38885</v>
       </c>
@@ -12910,7 +12963,7 @@
         <v>198.42</v>
       </c>
     </row>
-    <row r="363" spans="1:10">
+    <row r="363" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A363" s="3">
         <v>38885</v>
       </c>
@@ -12942,7 +12995,7 @@
         <v>140.37</v>
       </c>
     </row>
-    <row r="364" spans="1:10">
+    <row r="364" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A364" s="3">
         <v>38885</v>
       </c>
@@ -12974,7 +13027,7 @@
         <v>105.91</v>
       </c>
     </row>
-    <row r="365" spans="1:10">
+    <row r="365" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A365" s="3">
         <v>38885</v>
       </c>
@@ -13006,7 +13059,7 @@
         <v>101.46</v>
       </c>
     </row>
-    <row r="366" spans="1:10">
+    <row r="366" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A366" s="3">
         <v>38886</v>
       </c>
@@ -13038,7 +13091,7 @@
         <v>180.25</v>
       </c>
     </row>
-    <row r="367" spans="1:10">
+    <row r="367" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A367" s="3">
         <v>38886</v>
       </c>
@@ -13070,7 +13123,7 @@
         <v>112.74</v>
       </c>
     </row>
-    <row r="368" spans="1:10">
+    <row r="368" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A368" s="3">
         <v>38886</v>
       </c>
@@ -13102,7 +13155,7 @@
         <v>96.42</v>
       </c>
     </row>
-    <row r="369" spans="1:10">
+    <row r="369" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A369" s="3">
         <v>38886</v>
       </c>
@@ -13134,7 +13187,7 @@
         <v>210.29</v>
       </c>
     </row>
-    <row r="370" spans="1:10">
+    <row r="370" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A370" s="3">
         <v>38887</v>
       </c>
@@ -13166,7 +13219,7 @@
         <v>109.08</v>
       </c>
     </row>
-    <row r="371" spans="1:10">
+    <row r="371" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A371" s="3">
         <v>38887</v>
       </c>
@@ -13198,7 +13251,7 @@
         <v>180.01</v>
       </c>
     </row>
-    <row r="372" spans="1:10">
+    <row r="372" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A372" s="3">
         <v>38887</v>
       </c>
@@ -13230,7 +13283,7 @@
         <v>56.92</v>
       </c>
     </row>
-    <row r="373" spans="1:10">
+    <row r="373" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A373" s="3">
         <v>38887</v>
       </c>
@@ -13262,7 +13315,7 @@
         <v>77.489999999999995</v>
       </c>
     </row>
-    <row r="374" spans="1:10">
+    <row r="374" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A374" s="3">
         <v>38887</v>
       </c>
@@ -13294,7 +13347,7 @@
         <v>161.16</v>
       </c>
     </row>
-    <row r="375" spans="1:10">
+    <row r="375" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A375" s="3">
         <v>38887</v>
       </c>
@@ -13326,7 +13379,7 @@
         <v>110.87</v>
       </c>
     </row>
-    <row r="376" spans="1:10">
+    <row r="376" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A376" s="3">
         <v>38887</v>
       </c>
@@ -13358,7 +13411,7 @@
         <v>64.95</v>
       </c>
     </row>
-    <row r="377" spans="1:10">
+    <row r="377" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A377" s="3">
         <v>38888</v>
       </c>
@@ -13390,7 +13443,7 @@
         <v>108.18</v>
       </c>
     </row>
-    <row r="378" spans="1:10">
+    <row r="378" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A378" s="3">
         <v>38888</v>
       </c>
@@ -13422,7 +13475,7 @@
         <v>154.22</v>
       </c>
     </row>
-    <row r="379" spans="1:10">
+    <row r="379" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A379" s="3">
         <v>38888</v>
       </c>
@@ -13454,7 +13507,7 @@
         <v>129.43</v>
       </c>
     </row>
-    <row r="380" spans="1:10">
+    <row r="380" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A380" s="3">
         <v>38889</v>
       </c>
@@ -13486,7 +13539,7 @@
         <v>60.16</v>
       </c>
     </row>
-    <row r="381" spans="1:10">
+    <row r="381" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A381" s="3">
         <v>38889</v>
       </c>
@@ -13518,7 +13571,7 @@
         <v>357.67</v>
       </c>
     </row>
-    <row r="382" spans="1:10">
+    <row r="382" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A382" s="3">
         <v>38889</v>
       </c>
@@ -13550,7 +13603,7 @@
         <v>218.01</v>
       </c>
     </row>
-    <row r="383" spans="1:10">
+    <row r="383" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A383" s="3">
         <v>38890</v>
       </c>
@@ -13582,7 +13635,7 @@
         <v>250.51</v>
       </c>
     </row>
-    <row r="384" spans="1:10">
+    <row r="384" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A384" s="3">
         <v>38890</v>
       </c>
@@ -13614,7 +13667,7 @@
         <v>106.25</v>
       </c>
     </row>
-    <row r="385" spans="1:10">
+    <row r="385" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A385" s="3">
         <v>38890</v>
       </c>
@@ -13646,7 +13699,7 @@
         <v>64.52</v>
       </c>
     </row>
-    <row r="386" spans="1:10">
+    <row r="386" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A386" s="3">
         <v>38890</v>
       </c>
@@ -13678,7 +13731,7 @@
         <v>78.34</v>
       </c>
     </row>
-    <row r="387" spans="1:10">
+    <row r="387" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A387" s="3">
         <v>38890</v>
       </c>
@@ -13710,7 +13763,7 @@
         <v>70.05</v>
       </c>
     </row>
-    <row r="388" spans="1:10">
+    <row r="388" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A388" s="3">
         <v>38890</v>
       </c>
@@ -13742,7 +13795,7 @@
         <v>119.42</v>
       </c>
     </row>
-    <row r="389" spans="1:10">
+    <row r="389" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A389" s="3">
         <v>38890</v>
       </c>
@@ -13774,7 +13827,7 @@
         <v>169.63</v>
       </c>
     </row>
-    <row r="390" spans="1:10">
+    <row r="390" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A390" s="3">
         <v>38891</v>
       </c>
@@ -13806,7 +13859,7 @@
         <v>188.26</v>
       </c>
     </row>
-    <row r="391" spans="1:10">
+    <row r="391" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A391" s="3">
         <v>38891</v>
       </c>
@@ -13838,7 +13891,7 @@
         <v>161.86000000000001</v>
       </c>
     </row>
-    <row r="392" spans="1:10">
+    <row r="392" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A392" s="3">
         <v>38891</v>
       </c>
@@ -13870,7 +13923,7 @@
         <v>333.4</v>
       </c>
     </row>
-    <row r="393" spans="1:10">
+    <row r="393" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A393" s="3">
         <v>38892</v>
       </c>
@@ -13902,7 +13955,7 @@
         <v>124.58</v>
       </c>
     </row>
-    <row r="394" spans="1:10">
+    <row r="394" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A394" s="3">
         <v>38892</v>
       </c>
@@ -13934,7 +13987,7 @@
         <v>170.64</v>
       </c>
     </row>
-    <row r="395" spans="1:10">
+    <row r="395" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A395" s="3">
         <v>38892</v>
       </c>
@@ -13966,7 +14019,7 @@
         <v>138.38</v>
       </c>
     </row>
-    <row r="396" spans="1:10">
+    <row r="396" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A396" s="3">
         <v>38892</v>
       </c>
@@ -13998,7 +14051,7 @@
         <v>96.05</v>
       </c>
     </row>
-    <row r="397" spans="1:10">
+    <row r="397" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A397" s="3">
         <v>38892</v>
       </c>
@@ -14030,7 +14083,7 @@
         <v>142.97999999999999</v>
       </c>
     </row>
-    <row r="398" spans="1:10">
+    <row r="398" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A398" s="3">
         <v>38892</v>
       </c>
@@ -14062,7 +14115,7 @@
         <v>185.98</v>
       </c>
     </row>
-    <row r="399" spans="1:10">
+    <row r="399" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A399" s="3">
         <v>38893</v>
       </c>
@@ -14094,7 +14147,7 @@
         <v>111.67</v>
       </c>
     </row>
-    <row r="400" spans="1:10">
+    <row r="400" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A400" s="3">
         <v>38893</v>
       </c>
@@ -14126,7 +14179,7 @@
         <v>170.13</v>
       </c>
     </row>
-    <row r="401" spans="1:10">
+    <row r="401" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A401" s="3">
         <v>38893</v>
       </c>
@@ -14158,7 +14211,7 @@
         <v>80.08</v>
       </c>
     </row>
-    <row r="402" spans="1:10">
+    <row r="402" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A402" s="3">
         <v>38893</v>
       </c>
@@ -14190,7 +14243,7 @@
         <v>180.66</v>
       </c>
     </row>
-    <row r="403" spans="1:10">
+    <row r="403" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A403" s="3">
         <v>38893</v>
       </c>
@@ -14222,7 +14275,7 @@
         <v>85.79</v>
       </c>
     </row>
-    <row r="404" spans="1:10">
+    <row r="404" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A404" s="3">
         <v>38893</v>
       </c>
@@ -14261,12 +14314,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>